<commit_message>
bijwerken logboek + planning
</commit_message>
<xml_diff>
--- a/gekregen documentatie/20160920_sjabloon agenda.xlsx
+++ b/gekregen documentatie/20160920_sjabloon agenda.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2016-2017\Periode 5\Barroc-IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - ROC West-Brabant\Periode_5\project\ObesiCodeDocs\gekregen documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="D244A484B8B42A6CA35EBCC7D9900F4E1D13FEFC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="11760"/>
+    <workbookView minimized="1" xWindow="240" yWindow="90" windowWidth="19440" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Fer</author>
     <author>Fer Krimpen</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -35,7 +36,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fer:</t>
         </r>
@@ -44,14 +45,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vul hier onderwerp (bijv. Naam Project) en groepsnummer in.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fer:</t>
         </r>
@@ -68,14 +69,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vul hier ook eindtijd in. Bepaal deze a.d.h.v. cel C18.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="1" shapeId="0">
+    <comment ref="H18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fer Krimpen:</t>
         </r>
@@ -92,14 +93,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vul hier ook de naam van je projectbegeleider in.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fer:</t>
         </r>
@@ -116,7 +117,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vul  hier ook de naam van je projectbegeleider  in.</t>
@@ -214,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
@@ -286,14 +287,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -587,20 +588,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,6 +599,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -706,6 +707,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -741,6 +759,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -916,7 +951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -926,23 +961,23 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.86328125" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.265625" customWidth="1"/>
-    <col min="8" max="8" width="34.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.73046875" customWidth="1"/>
-    <col min="10" max="10" width="5.59765625" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="52"/>
       <c r="C2" s="53"/>
       <c r="D2" s="53"/>
@@ -952,45 +987,45 @@
       <c r="H2" s="54"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="55" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B4" s="58" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1043,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14"/>
@@ -1018,7 +1053,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
@@ -1035,7 +1070,7 @@
       <c r="I8" s="19"/>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
@@ -1050,7 +1085,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="22" t="s">
@@ -1066,7 +1101,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="22"/>
@@ -1077,7 +1112,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="22"/>
@@ -1089,7 +1124,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="22"/>
@@ -1101,7 +1136,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="22"/>
@@ -1113,7 +1148,7 @@
       <c r="H14" s="25"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="22" t="s">
@@ -1129,7 +1164,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
       <c r="C16" s="13"/>
       <c r="D16" s="22" t="s">
@@ -1145,7 +1180,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -1154,7 +1189,7 @@
       <c r="G17" s="30"/>
       <c r="H17" s="31"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="33">
         <f>SUM(C8:C17)</f>
@@ -1172,7 +1207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="37"/>
       <c r="C19" s="33"/>
       <c r="D19" s="38" t="s">
@@ -1187,7 +1222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="37"/>
       <c r="C20" s="33"/>
       <c r="D20" s="38" t="s">
@@ -1200,7 +1235,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="40"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="37"/>
       <c r="C21" s="33"/>
       <c r="D21" s="38" t="s">
@@ -1213,7 +1248,7 @@
       <c r="G21" s="39"/>
       <c r="H21" s="40"/>
     </row>
-    <row r="22" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
       <c r="D22" s="43" t="s">
@@ -1226,12 +1261,12 @@
       <c r="G22" s="45"/>
       <c r="H22" s="46"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="47"/>
       <c r="E25" s="4">
         <v>1</v>
@@ -1239,7 +1274,7 @@
       <c r="F25" s="48"/>
       <c r="I25" s="49"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="E26" s="4">
         <v>2</v>
@@ -1247,7 +1282,7 @@
       <c r="F26" s="21"/>
       <c r="I26" s="49"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="E27" s="4">
         <v>3</v>
@@ -1255,7 +1290,7 @@
       <c r="F27" s="23"/>
       <c r="I27" s="49"/>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4">
@@ -1266,14 +1301,14 @@
       <c r="H28" s="50"/>
       <c r="I28" s="51"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="E29" s="4">
         <v>5</v>
       </c>
       <c r="I29" s="49"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="E30" s="4">
         <v>6</v>
@@ -1281,7 +1316,7 @@
       <c r="F30" s="48"/>
       <c r="I30" s="49"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="E31" s="4">
         <v>7</v>
@@ -1289,18 +1324,18 @@
       <c r="F31" s="48"/>
       <c r="I31" s="49"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="F32" s="48"/>
       <c r="I32" s="49"/>
     </row>
-    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="49"/>
     </row>
-    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="4">
         <v>1</v>
       </c>
@@ -1310,7 +1345,7 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="4">
         <v>2</v>
       </c>
@@ -1320,7 +1355,7 @@
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
     </row>
-    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="4">
         <v>3</v>
       </c>
@@ -1329,76 +1364,76 @@
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
     </row>
-    <row r="37" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I60" s="5"/>
     </row>
   </sheetData>
@@ -1416,42 +1451,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1504,23 +1539,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>